<commit_message>
Update SWB_modeling_utils with corrected fitting fns
</commit_message>
<xml_diff>
--- a/figs/models_summary.xlsx
+++ b/figs/models_summary.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrafink/Documents/GraduateSchool/SaezLab/SWB/swb_computational_modeling/figs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandrafink/Documents/GraduateSchool/SaezLab/SWB/swb_computational_modeling/swb_behav_models/figs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B4908C-8691-174C-932D-D425E6ED1A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903F1982-7F18-E643-A004-0560CC859219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="760" windowWidth="27120" windowHeight="17700" xr2:uid="{C765D490-1C17-474E-9F19-B8C80CB7CBF8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="011424" sheetId="2" r:id="rId1"/>
+    <sheet name="091123" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -124,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,7 +148,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,10 +614,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A390074-BEE3-0847-8A4A-C7D78D76F011}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F33FDB2-E1B6-9443-98D0-02DFFB38845E}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+    <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -770,7 +782,7 @@
         <v>4.49</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>

</xml_diff>